<commit_message>
Sync data from OneDrive and add sync script (v10)
</commit_message>
<xml_diff>
--- a/step_data.xlsx.xlsx
+++ b/step_data.xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iCloud\iCloudDrive\Cursor\Alkoo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e189142475a5b38f/CURSOR/Alkoo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C473DBDE-0467-4BE0-8395-9F06306A6640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{C473DBDE-0467-4BE0-8395-9F06306A6640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A69B5872-1358-4DAB-875B-8BD31D17D813}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{80A7368D-0987-4F93-836C-3B46FCE69545}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{80A7368D-0987-4F93-836C-3B46FCE69545}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -3091,6 +3091,12 @@
                 <c:pt idx="2">
                   <c:v>7328</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>7998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8790</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3198,6 +3204,12 @@
                 <c:pt idx="2">
                   <c:v>17885</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>15789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3292,6 +3304,12 @@
                 <c:pt idx="2">
                   <c:v>7736</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>7493</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9106</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3386,6 +3404,12 @@
                 <c:pt idx="2">
                   <c:v>8418</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>6660</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3480,6 +3504,12 @@
                 <c:pt idx="2">
                   <c:v>5842</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>7425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7091</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3574,6 +3604,12 @@
                 <c:pt idx="2">
                   <c:v>6090</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>4936</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3668,6 +3704,12 @@
                 <c:pt idx="2">
                   <c:v>10333</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>9222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9135</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3848,6 +3890,12 @@
                   <c:v>2463</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2463</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2463</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2463</c:v>
                 </c:pt>
               </c:numCache>
@@ -3956,6 +4004,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1783</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1745</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5645,7 +5699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A173BF-8A83-4E52-A412-5058581D1F88}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5799,11 +5853,11 @@
       </c>
       <c r="W2" s="19">
         <f>'12月'!AH8</f>
-        <v>10333</v>
+        <v>9135</v>
       </c>
       <c r="X2" s="2">
         <f>AVERAGE(B2:W2)</f>
-        <v>5541.105263157895</v>
+        <v>5478.0526315789475</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.4">
@@ -5909,11 +5963,11 @@
       </c>
       <c r="W4" s="19">
         <f>'12月'!AH4</f>
-        <v>7736</v>
+        <v>9106</v>
       </c>
       <c r="X4" s="2">
         <f t="shared" si="0"/>
-        <v>7004.590909090909</v>
+        <v>7066.863636363636</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.4">
@@ -5986,11 +6040,11 @@
       </c>
       <c r="W5" s="19">
         <f>'12月'!AH5</f>
-        <v>8418</v>
+        <v>5740</v>
       </c>
       <c r="X5" s="2">
         <f t="shared" si="0"/>
-        <v>7175.272727272727</v>
+        <v>7053.545454545455</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.4">
@@ -6063,11 +6117,11 @@
       </c>
       <c r="W6" s="19">
         <f>'12月'!AH3</f>
-        <v>17885</v>
+        <v>15391</v>
       </c>
       <c r="X6" s="2">
         <f t="shared" si="0"/>
-        <v>7944.818181818182</v>
+        <v>7831.454545454545</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.4">
@@ -6140,11 +6194,11 @@
       </c>
       <c r="W7" s="19">
         <f>'12月'!AH2</f>
-        <v>7328</v>
+        <v>8790</v>
       </c>
       <c r="X7" s="2">
         <f t="shared" si="0"/>
-        <v>12831.181818181818</v>
+        <v>12897.636363636364</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.4">
@@ -6270,11 +6324,11 @@
       </c>
       <c r="W9" s="19">
         <f>'12月'!AH7</f>
-        <v>6090</v>
+        <v>6976</v>
       </c>
       <c r="X9" s="2">
         <f t="shared" si="0"/>
-        <v>6575.090909090909</v>
+        <v>6615.363636363636</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.4">
@@ -6323,11 +6377,11 @@
       </c>
       <c r="W10" s="19">
         <f>'12月'!AH11</f>
-        <v>1783</v>
+        <v>1888</v>
       </c>
       <c r="X10" s="2">
         <f t="shared" si="0"/>
-        <v>2116.7857142857142</v>
+        <v>2124.2857142857142</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.4">
@@ -6417,11 +6471,11 @@
       </c>
       <c r="W11" s="2">
         <f t="shared" si="2"/>
-        <v>6892.8888888888887</v>
+        <v>6609.8888888888887</v>
       </c>
       <c r="X11" s="2">
         <f>AVERAGE(B11:W11)</f>
-        <v>6795.2675736961455</v>
+        <v>6781.7913832199547</v>
       </c>
     </row>
   </sheetData>
@@ -7668,8 +7722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C3C389-DF96-44D4-A685-62AE24C5DF52}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7803,8 +7857,12 @@
       <c r="E2" s="13">
         <v>7328</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="F2" s="13">
+        <v>7998</v>
+      </c>
+      <c r="G2" s="13">
+        <v>8790</v>
+      </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -7833,7 +7891,7 @@
       <c r="AG2" s="14"/>
       <c r="AH2" s="17" cm="1">
         <f t="array" ref="AH2">LOOKUP(2,1/(ISNUMBER(C2:AG2)),C2:AG2)</f>
-        <v>7328</v>
+        <v>8790</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.4">
@@ -7852,8 +7910,12 @@
       <c r="E3" s="13">
         <v>17885</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="13">
+        <v>15789</v>
+      </c>
+      <c r="G3" s="13">
+        <v>15391</v>
+      </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -7882,7 +7944,7 @@
       <c r="AG3" s="14"/>
       <c r="AH3" s="17" cm="1">
         <f t="array" ref="AH3">LOOKUP(2,1/(ISNUMBER(C3:AG3)),C3:AG3)</f>
-        <v>17885</v>
+        <v>15391</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.4">
@@ -7901,8 +7963,12 @@
       <c r="E4" s="13">
         <v>7736</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="13">
+        <v>7493</v>
+      </c>
+      <c r="G4" s="13">
+        <v>9106</v>
+      </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -7931,7 +7997,7 @@
       <c r="AG4" s="14"/>
       <c r="AH4" s="17" cm="1">
         <f t="array" ref="AH4">LOOKUP(2,1/(ISNUMBER(C4:AG4)),C4:AG4)</f>
-        <v>7736</v>
+        <v>9106</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.4">
@@ -7950,8 +8016,12 @@
       <c r="E5" s="13">
         <v>8418</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="F5" s="13">
+        <v>6660</v>
+      </c>
+      <c r="G5" s="13">
+        <v>5740</v>
+      </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -7980,7 +8050,7 @@
       <c r="AG5" s="14"/>
       <c r="AH5" s="17" cm="1">
         <f t="array" ref="AH5">LOOKUP(2,1/(ISNUMBER(C5:AG5)),C5:AG5)</f>
-        <v>8418</v>
+        <v>5740</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.4">
@@ -7999,8 +8069,12 @@
       <c r="E6" s="13">
         <v>5842</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="13">
+        <v>7425</v>
+      </c>
+      <c r="G6" s="13">
+        <v>7091</v>
+      </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -8029,7 +8103,7 @@
       <c r="AG6" s="14"/>
       <c r="AH6" s="17" cm="1">
         <f t="array" ref="AH6">LOOKUP(2,1/(ISNUMBER(C6:AG6)),C6:AG6)</f>
-        <v>5842</v>
+        <v>7091</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.4">
@@ -8048,8 +8122,12 @@
       <c r="E7" s="13">
         <v>6090</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="13">
+        <v>4936</v>
+      </c>
+      <c r="G7" s="13">
+        <v>6976</v>
+      </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -8078,7 +8156,7 @@
       <c r="AG7" s="14"/>
       <c r="AH7" s="17" cm="1">
         <f t="array" ref="AH7">LOOKUP(2,1/(ISNUMBER(C7:AG7)),C7:AG7)</f>
-        <v>6090</v>
+        <v>6976</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.4">
@@ -8097,8 +8175,12 @@
       <c r="E8" s="13">
         <v>10333</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="13">
+        <v>9222</v>
+      </c>
+      <c r="G8" s="13">
+        <v>9135</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -8127,7 +8209,7 @@
       <c r="AG8" s="14"/>
       <c r="AH8" s="17" cm="1">
         <f t="array" ref="AH8">LOOKUP(2,1/(ISNUMBER(C8:AG8)),C8:AG8)</f>
-        <v>10333</v>
+        <v>9135</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.4">
@@ -8191,8 +8273,12 @@
       <c r="E10" s="13">
         <v>2463</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="13">
+        <v>2463</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2463</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -8240,8 +8326,12 @@
       <c r="E11" s="13">
         <v>1783</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="13">
+        <v>1745</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1888</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -8270,7 +8360,7 @@
       <c r="AG11" s="14"/>
       <c r="AH11" s="17" cm="1">
         <f t="array" ref="AH11">LOOKUP(2,1/(ISNUMBER(C11:AG11)),C11:AG11)</f>
-        <v>1783</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.4">

</xml_diff>